<commit_message>
exercie avion en cours
</commit_message>
<xml_diff>
--- a/03-Databases/exerciceSQL/courses_de_chevaux/courses_de_chevaux.xlsx
+++ b/03-Databases/exerciceSQL/courses_de_chevaux/courses_de_chevaux.xlsx
@@ -1,14 +1,23 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr defaultThemeVersion="164011"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="28227"/>
+  <workbookPr/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\bherault\Documents\GitHub\DWWM_2409_HB\03-Databases\exerciceSQL\courses_de_chevaux\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1B03B82A-85CD-46DE-80C5-894F91BC39A5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Feuil1" sheetId="1" r:id="rId1"/>
   </sheets>
+  <definedNames>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Feuil1!$C$2:$K$2</definedName>
+  </definedNames>
   <calcPr calcId="162913"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
@@ -18,15 +27,56 @@
 </workbook>
 </file>
 
+<file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="19" uniqueCount="10">
+  <si>
+    <t>course_id</t>
+  </si>
+  <si>
+    <t>course_nom</t>
+  </si>
+  <si>
+    <t xml:space="preserve">course_date </t>
+  </si>
+  <si>
+    <t>cheval_id</t>
+  </si>
+  <si>
+    <t>cheval_numero</t>
+  </si>
+  <si>
+    <t>cheval_nom</t>
+  </si>
+  <si>
+    <t xml:space="preserve">cheval_arrive </t>
+  </si>
+  <si>
+    <t>paris_id</t>
+  </si>
+  <si>
+    <t xml:space="preserve">paris_type </t>
+  </si>
+  <si>
+    <t>Colonne1</t>
+  </si>
+</sst>
+</file>
+
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="1" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="12"/>
+      <name val="Aptos"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="2">
@@ -37,7 +87,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="1">
+  <borders count="3">
     <border>
       <left/>
       <right/>
@@ -45,17 +95,159 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="medium">
+        <color rgb="FF156082"/>
+      </left>
+      <right style="medium">
+        <color rgb="FF156082"/>
+      </right>
+      <top style="medium">
+        <color rgb="FF156082"/>
+      </top>
+      <bottom style="medium">
+        <color rgb="FF156082"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color rgb="FF45B0E1"/>
+      </left>
+      <right style="medium">
+        <color rgb="FF45B0E1"/>
+      </right>
+      <top/>
+      <bottom style="medium">
+        <color rgb="FF45B0E1"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="0"/>
+  <dxfs count="12">
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="12"/>
+        <color auto="1"/>
+        <name val="Aptos"/>
+        <family val="2"/>
+        <scheme val="none"/>
+      </font>
+      <fill>
+        <patternFill patternType="none">
+          <fgColor indexed="64"/>
+          <bgColor indexed="65"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="general" vertical="top" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left style="medium">
+          <color rgb="FF45B0E1"/>
+        </left>
+        <right style="medium">
+          <color rgb="FF45B0E1"/>
+        </right>
+        <top/>
+        <bottom/>
+      </border>
+    </dxf>
+    <dxf>
+      <alignment horizontal="general" vertical="top" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="general" vertical="top" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="general" vertical="top" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="general" vertical="top" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="general" vertical="top" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="general" vertical="top" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="general" vertical="top" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="general" vertical="top" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="general" vertical="top" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="general" vertical="top" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="12"/>
+        <color auto="1"/>
+        <name val="Aptos"/>
+        <family val="2"/>
+        <scheme val="none"/>
+      </font>
+      <fill>
+        <patternFill patternType="none">
+          <fgColor indexed="64"/>
+          <bgColor indexed="65"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="general" vertical="top" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="medium">
+          <color rgb="FF45B0E1"/>
+        </left>
+        <right style="medium">
+          <color rgb="FF45B0E1"/>
+        </right>
+        <top/>
+        <bottom style="medium">
+          <color rgb="FF45B0E1"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+  </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
@@ -66,6 +258,25 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{B7DC2B8C-D7A8-4950-80A4-1B9663BBA2AD}" name="Tableau1" displayName="Tableau1" ref="B2:K13" totalsRowShown="0" headerRowDxfId="0" dataDxfId="1">
+  <autoFilter ref="B2:K13" xr:uid="{B7DC2B8C-D7A8-4950-80A4-1B9663BBA2AD}"/>
+  <tableColumns count="10">
+    <tableColumn id="1" xr3:uid="{07A3D074-6C9E-4562-B4F2-AAA039A37314}" name="Colonne1" dataDxfId="11"/>
+    <tableColumn id="2" xr3:uid="{022D19E4-C8F9-4867-87A4-FA2272A75E35}" name="course_id" dataDxfId="10"/>
+    <tableColumn id="3" xr3:uid="{A88F01C1-8598-4B70-90DA-BA8A19E8253C}" name="course_nom" dataDxfId="9"/>
+    <tableColumn id="4" xr3:uid="{69B9F6F0-CB3D-4BAF-AF5E-D09BE655B258}" name="course_date " dataDxfId="8"/>
+    <tableColumn id="5" xr3:uid="{5A95F468-7AD0-4AE3-A61B-31A12AD7A2C2}" name="cheval_id" dataDxfId="7"/>
+    <tableColumn id="6" xr3:uid="{17E13F12-4D81-4B75-A191-E4CC4F837B6A}" name="cheval_numero" dataDxfId="6"/>
+    <tableColumn id="7" xr3:uid="{668877FC-030E-4E6A-BA46-A6BDB1210874}" name="cheval_nom" dataDxfId="5"/>
+    <tableColumn id="8" xr3:uid="{E7F066D1-52B1-4512-AFD3-92A5C0660E08}" name="cheval_arrive " dataDxfId="4"/>
+    <tableColumn id="9" xr3:uid="{524C19A7-D71B-4F1F-AC73-DE5382C9DBCF}" name="paris_id" dataDxfId="3"/>
+    <tableColumn id="10" xr3:uid="{53F90FC3-2D95-4494-8EC3-6240E3B36135}" name="paris_type " dataDxfId="2"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -330,13 +541,226 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="B1:K13"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="N11" sqref="N11"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <sheetData/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="2" max="2" width="20.140625" customWidth="1"/>
+    <col min="3" max="3" width="13.5703125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="16.28515625" hidden="1" customWidth="1"/>
+    <col min="5" max="5" width="16.42578125" hidden="1" customWidth="1"/>
+    <col min="6" max="6" width="13.42578125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="19.7109375" hidden="1" customWidth="1"/>
+    <col min="8" max="8" width="16.140625" hidden="1" customWidth="1"/>
+    <col min="9" max="9" width="17.5703125" hidden="1" customWidth="1"/>
+    <col min="10" max="10" width="11.5703125" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="14.28515625" hidden="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="2:11" ht="46.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="2" spans="2:11" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B2" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="C2" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="D2" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="E2" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="F2" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="G2" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="H2" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="I2" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="J2" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="K2" s="3" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="3" spans="2:11" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B3" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="C3" s="1"/>
+      <c r="D3" s="1"/>
+      <c r="E3" s="1"/>
+      <c r="F3" s="1"/>
+      <c r="G3" s="1"/>
+      <c r="H3" s="1"/>
+      <c r="I3" s="1"/>
+      <c r="J3" s="1"/>
+      <c r="K3" s="1"/>
+    </row>
+    <row r="4" spans="2:11" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B4" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="C4" s="1">
+        <v>1</v>
+      </c>
+      <c r="D4" s="1"/>
+      <c r="E4" s="1"/>
+      <c r="F4" s="1"/>
+      <c r="G4" s="1"/>
+      <c r="H4" s="1"/>
+      <c r="I4" s="1"/>
+      <c r="J4" s="1"/>
+      <c r="K4" s="1"/>
+    </row>
+    <row r="5" spans="2:11" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B5" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="C5" s="1">
+        <v>1</v>
+      </c>
+      <c r="D5" s="1"/>
+      <c r="E5" s="1"/>
+      <c r="F5" s="1"/>
+      <c r="G5" s="1"/>
+      <c r="H5" s="1"/>
+      <c r="I5" s="1"/>
+      <c r="J5" s="1"/>
+      <c r="K5" s="1"/>
+    </row>
+    <row r="6" spans="2:11" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B6" s="3"/>
+      <c r="C6" s="1"/>
+      <c r="D6" s="1"/>
+      <c r="E6" s="1"/>
+      <c r="F6" s="1"/>
+      <c r="G6" s="1"/>
+      <c r="H6" s="1"/>
+      <c r="I6" s="1"/>
+      <c r="J6" s="1"/>
+      <c r="K6" s="1"/>
+    </row>
+    <row r="7" spans="2:11" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B7" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="C7" s="1"/>
+      <c r="D7" s="1"/>
+      <c r="E7" s="1"/>
+      <c r="F7" s="1"/>
+      <c r="G7" s="1"/>
+      <c r="H7" s="1"/>
+      <c r="I7" s="1"/>
+      <c r="J7" s="1"/>
+      <c r="K7" s="1"/>
+    </row>
+    <row r="8" spans="2:11" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B8" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="C8" s="1"/>
+      <c r="D8" s="1"/>
+      <c r="E8" s="1"/>
+      <c r="F8" s="1">
+        <v>1</v>
+      </c>
+      <c r="G8" s="1"/>
+      <c r="H8" s="1"/>
+      <c r="I8" s="1"/>
+      <c r="J8" s="1"/>
+      <c r="K8" s="1"/>
+    </row>
+    <row r="9" spans="2:11" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B9" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="C9" s="1"/>
+      <c r="D9" s="1"/>
+      <c r="E9" s="1"/>
+      <c r="F9" s="1">
+        <v>1</v>
+      </c>
+      <c r="G9" s="1"/>
+      <c r="H9" s="1"/>
+      <c r="I9" s="1"/>
+      <c r="J9" s="1"/>
+      <c r="K9" s="1"/>
+    </row>
+    <row r="10" spans="2:11" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B10" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="C10" s="1"/>
+      <c r="D10" s="1"/>
+      <c r="E10" s="1"/>
+      <c r="F10" s="1">
+        <v>1</v>
+      </c>
+      <c r="G10" s="1"/>
+      <c r="H10" s="1"/>
+      <c r="I10" s="1"/>
+      <c r="J10" s="1"/>
+      <c r="K10" s="1"/>
+    </row>
+    <row r="11" spans="2:11" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B11" s="3"/>
+      <c r="C11" s="1"/>
+      <c r="D11" s="1"/>
+      <c r="E11" s="1"/>
+      <c r="F11" s="1"/>
+      <c r="G11" s="1"/>
+      <c r="H11" s="1"/>
+      <c r="I11" s="1"/>
+      <c r="J11" s="1"/>
+      <c r="K11" s="1"/>
+    </row>
+    <row r="12" spans="2:11" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B12" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="C12" s="1"/>
+      <c r="D12" s="1"/>
+      <c r="E12" s="1"/>
+      <c r="F12" s="1"/>
+      <c r="G12" s="1"/>
+      <c r="H12" s="1"/>
+      <c r="I12" s="1"/>
+      <c r="J12" s="1"/>
+      <c r="K12" s="1"/>
+    </row>
+    <row r="13" spans="2:11" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B13" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="C13" s="1"/>
+      <c r="D13" s="1"/>
+      <c r="E13" s="1"/>
+      <c r="F13" s="1"/>
+      <c r="G13" s="1"/>
+      <c r="H13" s="1"/>
+      <c r="I13" s="1"/>
+      <c r="J13" s="1">
+        <v>1</v>
+      </c>
+      <c r="K13" s="1"/>
+    </row>
+  </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <tableParts count="1">
+    <tablePart r:id="rId1"/>
+  </tableParts>
 </worksheet>
 </file>
</xml_diff>